<commit_message>
Convertir archivos a Base64
</commit_message>
<xml_diff>
--- a/Documentos/Lista de checkeo.xlsx
+++ b/Documentos/Lista de checkeo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\iwana-sinergia\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707371CE-E671-40DF-B8DF-A86B3E0DD3F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E689F794-20A4-415B-9B41-CC170B49D3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -237,12 +237,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -272,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,12 +290,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,7 +580,7 @@
   <dimension ref="C2:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H50"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +608,7 @@
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>62</v>
       </c>
     </row>
@@ -610,13 +617,13 @@
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -628,7 +635,7 @@
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
@@ -638,19 +645,19 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="5"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="3" t="s">
         <v>11</v>
       </c>
@@ -660,7 +667,7 @@
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -672,7 +679,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="5"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
@@ -682,7 +689,7 @@
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="3" t="s">
         <v>14</v>
       </c>
@@ -692,7 +699,7 @@
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
@@ -702,7 +709,7 @@
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="5"/>
+      <c r="C12" s="6"/>
       <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
@@ -712,7 +719,7 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
@@ -724,7 +731,7 @@
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="5"/>
+      <c r="C14" s="6"/>
       <c r="D14" s="3" t="s">
         <v>20</v>
       </c>
@@ -734,7 +741,7 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
+      <c r="C15" s="6"/>
       <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
@@ -744,7 +751,7 @@
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
+      <c r="C16" s="6"/>
       <c r="D16" s="3" t="s">
         <v>22</v>
       </c>
@@ -754,7 +761,7 @@
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
       <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
@@ -764,7 +771,7 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
+      <c r="C18" s="6"/>
       <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
@@ -774,7 +781,7 @@
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="3" t="s">
         <v>25</v>
       </c>
@@ -784,7 +791,7 @@
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="5"/>
+      <c r="C20" s="6"/>
       <c r="D20" s="3" t="s">
         <v>26</v>
       </c>
@@ -794,7 +801,7 @@
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
+      <c r="C21" s="6"/>
       <c r="D21" s="3" t="s">
         <v>27</v>
       </c>
@@ -804,7 +811,7 @@
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="3" t="s">
         <v>28</v>
       </c>
@@ -814,7 +821,7 @@
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="3" t="s">
         <v>29</v>
       </c>
@@ -824,7 +831,7 @@
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -836,7 +843,7 @@
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="3" t="s">
         <v>31</v>
       </c>
@@ -846,7 +853,7 @@
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" s="5"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="3" t="s">
         <v>32</v>
       </c>
@@ -856,7 +863,7 @@
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="3" t="s">
         <v>33</v>
       </c>
@@ -866,7 +873,7 @@
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -878,7 +885,7 @@
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="3" t="s">
         <v>37</v>
       </c>
@@ -888,7 +895,7 @@
       <c r="H29" s="3"/>
     </row>
     <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C30" s="5"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="3" t="s">
         <v>36</v>
       </c>
@@ -898,7 +905,7 @@
       <c r="H30" s="3"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="3" t="s">
@@ -910,7 +917,7 @@
       <c r="H31" s="3"/>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" s="5"/>
+      <c r="C32" s="6"/>
       <c r="D32" s="3" t="s">
         <v>40</v>
       </c>
@@ -920,7 +927,7 @@
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
+      <c r="C33" s="6"/>
       <c r="D33" s="3" t="s">
         <v>41</v>
       </c>
@@ -930,7 +937,7 @@
       <c r="H33" s="3"/>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C34" s="5"/>
+      <c r="C34" s="6"/>
       <c r="D34" s="3" t="s">
         <v>42</v>
       </c>
@@ -940,7 +947,7 @@
       <c r="H34" s="3"/>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
+      <c r="C35" s="6"/>
       <c r="D35" s="3" t="s">
         <v>43</v>
       </c>
@@ -950,7 +957,7 @@
       <c r="H35" s="3"/>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
+      <c r="C36" s="6"/>
       <c r="D36" s="3" t="s">
         <v>44</v>
       </c>
@@ -960,7 +967,7 @@
       <c r="H36" s="3"/>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
+      <c r="C37" s="6"/>
       <c r="D37" s="3" t="s">
         <v>45</v>
       </c>
@@ -970,7 +977,7 @@
       <c r="H37" s="3"/>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="3" t="s">
         <v>46</v>
       </c>
@@ -980,7 +987,7 @@
       <c r="H38" s="3"/>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
+      <c r="C39" s="6"/>
       <c r="D39" s="3" t="s">
         <v>47</v>
       </c>
@@ -990,7 +997,7 @@
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
+      <c r="C40" s="6"/>
       <c r="D40" s="3" t="s">
         <v>48</v>
       </c>
@@ -1000,7 +1007,7 @@
       <c r="H40" s="3"/>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
+      <c r="C41" s="6"/>
       <c r="D41" s="3" t="s">
         <v>49</v>
       </c>
@@ -1010,7 +1017,7 @@
       <c r="H41" s="3"/>
     </row>
     <row r="42" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
+      <c r="C42" s="6"/>
       <c r="D42" s="3" t="s">
         <v>50</v>
       </c>
@@ -1020,7 +1027,7 @@
       <c r="H42" s="3"/>
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="3" t="s">
@@ -1032,7 +1039,7 @@
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C44" s="5"/>
+      <c r="C44" s="6"/>
       <c r="D44" s="3" t="s">
         <v>54</v>
       </c>
@@ -1042,7 +1049,7 @@
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="6" t="s">
         <v>55</v>
       </c>
       <c r="D45" s="3" t="s">
@@ -1054,7 +1061,7 @@
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C46" s="5"/>
+      <c r="C46" s="6"/>
       <c r="D46" s="3" t="s">
         <v>57</v>
       </c>
@@ -1064,7 +1071,7 @@
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
+      <c r="C47" s="6"/>
       <c r="D47" s="3" t="s">
         <v>58</v>
       </c>
@@ -1074,7 +1081,7 @@
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C48" s="5"/>
+      <c r="C48" s="6"/>
       <c r="D48" s="3" t="s">
         <v>59</v>
       </c>
@@ -1084,7 +1091,7 @@
       <c r="H48" s="3"/>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C49" s="5"/>
+      <c r="C49" s="6"/>
       <c r="D49" s="3" t="s">
         <v>60</v>
       </c>
@@ -1094,7 +1101,7 @@
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C50" s="5"/>
+      <c r="C50" s="6"/>
       <c r="D50" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>